<commit_message>
split user and dev readmes
</commit_message>
<xml_diff>
--- a/report-data-marts/monthly-milk-production/dummy-data/milk-prod-data-mart-reqs-1.5.xlsx
+++ b/report-data-marts/monthly-milk-production/dummy-data/milk-prod-data-mart-reqs-1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmartinez/Git/NASS-MILK/report-data-marts/monthly-milk-production/dummy-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6AF4D5-E38C-0448-A679-32C3ABBB7F70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9D2F83-2BF7-5343-9317-0A447A20E214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="16820" firstSheet="3" activeTab="11" xr2:uid="{18E74043-749A-FF40-A645-80F0F71A40CB}"/>
+    <workbookView xWindow="0" yWindow="3920" windowWidth="35840" windowHeight="18480" xr2:uid="{18E74043-749A-FF40-A645-80F0F71A40CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="91">
   <si>
     <t>Month</t>
   </si>
@@ -220,18 +220,6 @@
     <t>each row is an "entity" and each column is an "attribute" of that entity</t>
   </si>
   <si>
-    <t>If we assume they know how to manipulate tables we can give them one format and let them do the manipulation (I don't recommend this)</t>
-  </si>
-  <si>
-    <t>this will make the data auto-visualizable and auto-analyzable "out of the box" even for users who don't already know how to do tabular manipulations</t>
-  </si>
-  <si>
-    <t>I recommend including both the wide and long formats of every table in a release download</t>
-  </si>
-  <si>
-    <t>the tables are small enough that duplicating the data served shouldn't be a significant issue</t>
-  </si>
-  <si>
     <t>Read Me</t>
   </si>
   <si>
@@ -268,21 +256,6 @@
     <t>ENTITY</t>
   </si>
   <si>
-    <t>This isn't too different from the current QS which assumes users will "figure it out"</t>
-  </si>
-  <si>
-    <t>Another option is to give the users a choice between requesting either the long or the wide data and educating them on the difference</t>
-  </si>
-  <si>
-    <t>I also think this reduces our "eduational burden" because they can simply use the table they "like" and ignore the rest</t>
-  </si>
-  <si>
-    <t>We need to make a design decision about the minimum level of data manipulation and analysis skills we assume a user will have</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alterntively, we could educate them on when and how to pivot a long table to a wide one, and "melt" a wide table into a long one </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Note that the same data may be strucutured in different ways. </t>
     </r>
@@ -310,24 +283,6 @@
   </si>
   <si>
     <t>Dear Users,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I also don't recommend this because each tool will have their own idiosyncratic process which we either research and digest for them or abandon them to do it themselves</t>
-  </si>
-  <si>
-    <t>I also don't recommend this as it reminds me of requiring users to know the difference between survey and census before they can "just see" the data</t>
-  </si>
-  <si>
-    <t>Also, we would have to then manage the implementation of the choice at various "stops" along a user-journey.</t>
-  </si>
-  <si>
-    <t>Druid Team,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note that the data dictionary and actual data values in this sheet are merely "placeholders" </t>
-  </si>
-  <si>
-    <t>Eventually, someone, likely me, will need to create a "master data dictionary" and each data-mart can just pull the entries included in its use-case</t>
   </si>
   <si>
     <t>Description and Footnotes</t>
@@ -373,12 +328,6 @@
   </si>
   <si>
     <t>&lt;Report Month - 1&gt;</t>
-  </si>
-  <si>
-    <t>I would also like to add to our backlog, proposing upgrades to the reports</t>
-  </si>
-  <si>
-    <t>The layout is unituitive, sometimes line charts seem to have been placed amongts unrelated tables</t>
   </si>
   <si>
     <t>Easy for analysis where you want to compare one attribute to another grouped over the same entity</t>
@@ -4201,8 +4150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384B1D2C-4EE8-4143-A35F-EB382FB4A755}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4219,7 +4168,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -4266,7 +4215,7 @@
     <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -4296,7 +4245,7 @@
     <row r="6" spans="1:16" ht="31" x14ac:dyDescent="0.45">
       <c r="A6" s="9"/>
       <c r="B6" s="16" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -4345,7 +4294,7 @@
     <row r="9" spans="1:16" ht="26" x14ac:dyDescent="0.4">
       <c r="A9" s="9"/>
       <c r="B9" s="11" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -4356,7 +4305,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="N9" s="11" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
@@ -4398,32 +4347,32 @@
     <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="N12" s="17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="P12" s="20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.25">
@@ -4441,7 +4390,7 @@
         <v>2.6</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -4472,7 +4421,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -4503,7 +4452,7 @@
         <v>6.6</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -4583,17 +4532,13 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="26" x14ac:dyDescent="0.3">
-      <c r="B36" s="12" t="s">
-        <v>84</v>
-      </c>
+      <c r="B36" s="12"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:15" ht="26" x14ac:dyDescent="0.3">
-      <c r="B37" s="24" t="s">
-        <v>77</v>
-      </c>
+      <c r="B37" s="24"/>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
@@ -4605,31 +4550,23 @@
       <c r="E38" s="14"/>
     </row>
     <row r="39" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="C39" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="C39" s="15"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
     </row>
     <row r="40" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="C40" s="14"/>
-      <c r="D40" s="14" t="s">
-        <v>61</v>
-      </c>
+      <c r="D40" s="14"/>
       <c r="E40" s="14"/>
     </row>
     <row r="41" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="C41" s="14"/>
-      <c r="D41" s="14" t="s">
-        <v>59</v>
-      </c>
+      <c r="D41" s="14"/>
       <c r="E41" s="14"/>
     </row>
     <row r="42" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="C42" s="14"/>
-      <c r="D42" s="14" t="s">
-        <v>76</v>
-      </c>
+      <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="O42" s="7"/>
     </row>
@@ -4640,33 +4577,25 @@
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="C44" s="15" t="s">
-        <v>58</v>
-      </c>
+      <c r="C44" s="15"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
     </row>
     <row r="45" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="C45" s="14"/>
-      <c r="D45" s="14" t="s">
-        <v>74</v>
-      </c>
+      <c r="D45" s="14"/>
       <c r="E45" s="14"/>
     </row>
     <row r="46" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="C46" s="14"/>
-      <c r="D46" s="14" t="s">
-        <v>78</v>
-      </c>
+      <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="O46" s="7"/>
     </row>
     <row r="47" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="C47" s="15"/>
       <c r="D47" s="14"/>
-      <c r="E47" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="E47" s="14"/>
       <c r="O47" s="7"/>
     </row>
     <row r="48" spans="2:15" ht="21" x14ac:dyDescent="0.25">
@@ -4676,46 +4605,32 @@
       <c r="O48" s="7"/>
     </row>
     <row r="49" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="C49" s="15" t="s">
-        <v>75</v>
-      </c>
+      <c r="C49" s="15"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="O49" s="7"/>
     </row>
     <row r="50" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="D50" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="D50" s="14"/>
       <c r="M50" s="7"/>
     </row>
     <row r="51" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="D51" s="14" t="s">
-        <v>83</v>
-      </c>
+      <c r="D51" s="14"/>
     </row>
     <row r="54" spans="2:15" ht="26" x14ac:dyDescent="0.3">
-      <c r="B54" s="24" t="s">
-        <v>85</v>
-      </c>
+      <c r="B54" s="24"/>
     </row>
     <row r="56" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="C56" s="14" t="s">
-        <v>86</v>
-      </c>
+      <c r="C56" s="14"/>
     </row>
     <row r="58" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="C58" s="14"/>
     </row>
     <row r="59" spans="2:15" ht="26" x14ac:dyDescent="0.3">
-      <c r="B59" s="24" t="s">
-        <v>102</v>
-      </c>
+      <c r="B59" s="24"/>
     </row>
     <row r="61" spans="2:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="C61" s="14" t="s">
-        <v>103</v>
-      </c>
+      <c r="C61" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O13:O18 G47 D13:E15">
@@ -4832,7 +4747,7 @@
         <v>2033</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4861,7 +4776,7 @@
         <v>1925</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4890,7 +4805,7 @@
         <v>2084</v>
       </c>
       <c r="I4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4919,7 +4834,7 @@
         <v>2008</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4948,7 +4863,7 @@
         <v>2043</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4977,7 +4892,7 @@
         <v>1981</v>
       </c>
       <c r="I7" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -5006,7 +4921,7 @@
         <v>2016</v>
       </c>
       <c r="I8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5035,7 +4950,7 @@
         <v>2016</v>
       </c>
       <c r="I9" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5064,7 +4979,7 @@
         <v>2016</v>
       </c>
       <c r="I10" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5093,7 +5008,7 @@
         <v>2016</v>
       </c>
       <c r="I11" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5122,7 +5037,7 @@
         <v>2016</v>
       </c>
       <c r="I12" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5151,12 +5066,12 @@
         <v>2016</v>
       </c>
       <c r="I13" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B14" s="3">
         <v>16112800000</v>
@@ -5180,12 +5095,12 @@
         <v>1956.8</v>
       </c>
       <c r="I14" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B15" s="3">
         <v>16341600000</v>
@@ -5209,12 +5124,12 @@
         <v>1967.1</v>
       </c>
       <c r="I15" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B16" s="3">
         <v>16570400000</v>
@@ -5238,12 +5153,12 @@
         <v>1977.4</v>
       </c>
       <c r="I16" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3">
         <v>16799200000</v>
@@ -5267,12 +5182,12 @@
         <v>1987.7</v>
       </c>
       <c r="I17" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B18" s="3">
         <v>17699000000</v>
@@ -5296,12 +5211,12 @@
         <v>2033</v>
       </c>
       <c r="I18" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B19" s="3">
         <v>16132000000</v>
@@ -5325,12 +5240,12 @@
         <v>1925</v>
       </c>
       <c r="I19" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B20" s="3">
         <v>17916000000</v>
@@ -5354,12 +5269,12 @@
         <v>2084</v>
       </c>
       <c r="I20" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3">
         <v>17544000000</v>
@@ -5383,12 +5298,12 @@
         <v>2008</v>
       </c>
       <c r="I21" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3">
         <v>18137000000</v>
@@ -5412,12 +5327,12 @@
         <v>2043</v>
       </c>
       <c r="I22" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3">
         <v>18843000000</v>
@@ -5441,12 +5356,12 @@
         <v>2084.5</v>
       </c>
       <c r="I23" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B24" s="3">
         <v>19407300000</v>
@@ -5470,12 +5385,12 @@
         <v>2112.3000000000002</v>
       </c>
       <c r="I24" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B25" s="3">
         <v>19971600000</v>
@@ -5499,7 +5414,7 @@
         <v>2140.1</v>
       </c>
       <c r="I25" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -5574,7 +5489,7 @@
         <v>2019</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L2" s="27"/>
       <c r="M2" s="28"/>
@@ -5603,7 +5518,7 @@
         <v>2019</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L3" s="27"/>
       <c r="M3" s="28"/>
@@ -5632,7 +5547,7 @@
         <v>2019</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L4" s="27"/>
       <c r="M4" s="28"/>
@@ -5661,7 +5576,7 @@
         <v>2019</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L5" s="27"/>
       <c r="M5" s="28"/>
@@ -5690,7 +5605,7 @@
         <v>2019</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
@@ -5719,7 +5634,7 @@
         <v>2019</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L7" s="27"/>
       <c r="M7" s="28"/>
@@ -5748,7 +5663,7 @@
         <v>2019</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="28"/>
@@ -5777,7 +5692,7 @@
         <v>2019</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L9" s="27"/>
       <c r="M9" s="28"/>
@@ -5806,7 +5721,7 @@
         <v>2019</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
@@ -5835,7 +5750,7 @@
         <v>2019</v>
       </c>
       <c r="F11" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L11" s="27"/>
       <c r="M11" s="28"/>
@@ -5864,7 +5779,7 @@
         <v>2019</v>
       </c>
       <c r="F12" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L12" s="27"/>
       <c r="M12" s="28"/>
@@ -5893,7 +5808,7 @@
         <v>2019</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L13" s="27"/>
       <c r="M13" s="28"/>
@@ -5916,13 +5831,13 @@
         <v>1826.6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E14" s="31">
         <v>2019</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L14" s="27"/>
       <c r="M14" s="28"/>
@@ -5945,13 +5860,13 @@
         <v>1853.5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E15" s="31">
         <v>2019</v>
       </c>
       <c r="F15" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L15" s="27"/>
       <c r="M15" s="28"/>
@@ -5974,13 +5889,13 @@
         <v>1880.4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E16" s="31">
         <v>2019</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="28"/>
@@ -6003,13 +5918,13 @@
         <v>1907.3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E17" s="31">
         <v>2019</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L17" s="27"/>
       <c r="M17" s="28"/>
@@ -6032,13 +5947,13 @@
         <v>2010</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E18" s="31">
         <v>2019</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L18" s="27"/>
       <c r="M18" s="28"/>
@@ -6061,13 +5976,13 @@
         <v>1833</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E19" s="31">
         <v>2019</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L19" s="27"/>
       <c r="M19" s="28"/>
@@ -6090,13 +6005,13 @@
         <v>2038</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E20" s="31">
         <v>2019</v>
       </c>
       <c r="F20" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L20" s="27"/>
       <c r="M20" s="28"/>
@@ -6119,13 +6034,13 @@
         <v>1996</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E21" s="31">
         <v>2019</v>
       </c>
       <c r="F21" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L21" s="27"/>
       <c r="M21" s="28"/>
@@ -6148,13 +6063,13 @@
         <v>2063</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E22" s="31">
         <v>2019</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L22" s="27"/>
       <c r="M22" s="28"/>
@@ -6177,13 +6092,13 @@
         <v>2144.5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E23" s="31">
         <v>2019</v>
       </c>
       <c r="F23" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L23" s="27"/>
       <c r="M23" s="28"/>
@@ -6206,13 +6121,13 @@
         <v>2209.3000000000002</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E24" s="31">
         <v>2019</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L24" s="27"/>
       <c r="M24" s="28"/>
@@ -6235,13 +6150,13 @@
         <v>2274.1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E25" s="31">
         <v>2019</v>
       </c>
       <c r="F25" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="L25" s="27"/>
       <c r="M25" s="28"/>
@@ -6270,7 +6185,7 @@
         <v>2020</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -6290,7 +6205,7 @@
         <v>2020</v>
       </c>
       <c r="F27" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
@@ -6310,7 +6225,7 @@
         <v>2020</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
@@ -6330,7 +6245,7 @@
         <v>2020</v>
       </c>
       <c r="F29" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
@@ -6350,7 +6265,7 @@
         <v>2020</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -6370,7 +6285,7 @@
         <v>2020</v>
       </c>
       <c r="F31" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -6390,7 +6305,7 @@
         <v>2020</v>
       </c>
       <c r="F32" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -6410,7 +6325,7 @@
         <v>2020</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -6430,7 +6345,7 @@
         <v>2020</v>
       </c>
       <c r="F34" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -6450,7 +6365,7 @@
         <v>2020</v>
       </c>
       <c r="F35" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -6470,7 +6385,7 @@
         <v>2020</v>
       </c>
       <c r="F36" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -6490,7 +6405,7 @@
         <v>2020</v>
       </c>
       <c r="F37" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -6504,13 +6419,13 @@
         <v>1956.8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E38" s="31">
         <v>2020</v>
       </c>
       <c r="F38" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -6524,13 +6439,13 @@
         <v>1967.1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E39" s="31">
         <v>2020</v>
       </c>
       <c r="F39" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -6544,13 +6459,13 @@
         <v>1977.4</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E40" s="31">
         <v>2020</v>
       </c>
       <c r="F40" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -6564,13 +6479,13 @@
         <v>1987.7</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E41" s="31">
         <v>2020</v>
       </c>
       <c r="F41" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -6584,13 +6499,13 @@
         <v>2033</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E42" s="31">
         <v>2020</v>
       </c>
       <c r="F42" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -6604,13 +6519,13 @@
         <v>1925</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E43" s="31">
         <v>2020</v>
       </c>
       <c r="F43" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -6624,13 +6539,13 @@
         <v>2084</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E44" s="31">
         <v>2020</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -6644,13 +6559,13 @@
         <v>2008</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E45" s="31">
         <v>2020</v>
       </c>
       <c r="F45" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -6664,13 +6579,13 @@
         <v>2043</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E46" s="31">
         <v>2020</v>
       </c>
       <c r="F46" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -6684,13 +6599,13 @@
         <v>2084.5</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E47" s="31">
         <v>2020</v>
       </c>
       <c r="F47" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -6704,13 +6619,13 @@
         <v>2112.3000000000002</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E48" s="31">
         <v>2020</v>
       </c>
       <c r="F48" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -6724,13 +6639,13 @@
         <v>2140.1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E49" s="31">
         <v>2020</v>
       </c>
       <c r="F49" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -6750,7 +6665,7 @@
         <v>2019</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -6770,7 +6685,7 @@
         <v>2019</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -6790,7 +6705,7 @@
         <v>2019</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -6810,7 +6725,7 @@
         <v>2019</v>
       </c>
       <c r="F53" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -6830,7 +6745,7 @@
         <v>2019</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -6850,7 +6765,7 @@
         <v>2019</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -6870,7 +6785,7 @@
         <v>2019</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -6890,7 +6805,7 @@
         <v>2019</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -6910,7 +6825,7 @@
         <v>2019</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -6930,7 +6845,7 @@
         <v>2019</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -6950,7 +6865,7 @@
         <v>2019</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -6970,7 +6885,7 @@
         <v>2019</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -6984,13 +6899,13 @@
         <v>1826.6</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E62" s="31">
         <v>2019</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -7004,13 +6919,13 @@
         <v>1853.5</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E63" s="31">
         <v>2019</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -7024,13 +6939,13 @@
         <v>1880.4</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E64" s="31">
         <v>2019</v>
       </c>
       <c r="F64" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -7044,13 +6959,13 @@
         <v>1907.3</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E65" s="31">
         <v>2019</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -7064,13 +6979,13 @@
         <v>2010</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E66" s="31">
         <v>2019</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -7084,13 +6999,13 @@
         <v>1833</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E67" s="31">
         <v>2019</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -7104,13 +7019,13 @@
         <v>2038</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E68" s="31">
         <v>2019</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -7124,13 +7039,13 @@
         <v>1996</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E69" s="31">
         <v>2019</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -7144,13 +7059,13 @@
         <v>2063</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E70" s="31">
         <v>2019</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -7164,13 +7079,13 @@
         <v>2144.5</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E71" s="31">
         <v>2019</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -7184,13 +7099,13 @@
         <v>2209.3000000000002</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E72" s="31">
         <v>2019</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -7204,13 +7119,13 @@
         <v>2274.1</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E73" s="31">
         <v>2019</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -7230,7 +7145,7 @@
         <v>2020</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -7250,7 +7165,7 @@
         <v>2020</v>
       </c>
       <c r="F75" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -7270,7 +7185,7 @@
         <v>2020</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -7290,7 +7205,7 @@
         <v>2020</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -7310,7 +7225,7 @@
         <v>2020</v>
       </c>
       <c r="F78" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -7330,7 +7245,7 @@
         <v>2020</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -7350,7 +7265,7 @@
         <v>2020</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -7370,7 +7285,7 @@
         <v>2020</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -7390,7 +7305,7 @@
         <v>2020</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -7410,7 +7325,7 @@
         <v>2020</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -7430,7 +7345,7 @@
         <v>2020</v>
       </c>
       <c r="F84" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -7450,7 +7365,7 @@
         <v>2020</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -7464,13 +7379,13 @@
         <v>1956.8</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E86" s="31">
         <v>2020</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -7484,13 +7399,13 @@
         <v>1967.1</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E87" s="31">
         <v>2020</v>
       </c>
       <c r="F87" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -7504,13 +7419,13 @@
         <v>1977.4</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E88" s="31">
         <v>2020</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -7524,13 +7439,13 @@
         <v>1987.7</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E89" s="31">
         <v>2020</v>
       </c>
       <c r="F89" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -7544,13 +7459,13 @@
         <v>2033</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E90" s="31">
         <v>2020</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -7564,13 +7479,13 @@
         <v>1925</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E91" s="31">
         <v>2020</v>
       </c>
       <c r="F91" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -7584,13 +7499,13 @@
         <v>2084</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E92" s="31">
         <v>2020</v>
       </c>
       <c r="F92" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -7604,13 +7519,13 @@
         <v>2008</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E93" s="31">
         <v>2020</v>
       </c>
       <c r="F93" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -7624,13 +7539,13 @@
         <v>2043</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E94" s="31">
         <v>2020</v>
       </c>
       <c r="F94" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -7644,13 +7559,13 @@
         <v>2084.5</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E95" s="31">
         <v>2020</v>
       </c>
       <c r="F95" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -7664,13 +7579,13 @@
         <v>2112.3000000000002</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E96" s="31">
         <v>2020</v>
       </c>
       <c r="F96" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -7684,13 +7599,13 @@
         <v>2140.1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E97" s="31">
         <v>2020</v>
       </c>
       <c r="F97" s="25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -7702,7 +7617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF68689-30C7-074E-8257-973C71620241}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -7710,7 +7625,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>25</v>
@@ -7719,7 +7634,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
@@ -7762,7 +7677,7 @@
         <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>22</v>
@@ -9842,7 +9757,7 @@
         <v>2033</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -9871,7 +9786,7 @@
         <v>1925</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -9900,7 +9815,7 @@
         <v>2084</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -9929,7 +9844,7 @@
         <v>2008</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -9958,7 +9873,7 @@
         <v>2043</v>
       </c>
       <c r="I6" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -9987,7 +9902,7 @@
         <v>1981</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -10016,7 +9931,7 @@
         <v>2016</v>
       </c>
       <c r="I8" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -10045,7 +9960,7 @@
         <v>2016</v>
       </c>
       <c r="I9" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -10074,7 +9989,7 @@
         <v>2016</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -10103,7 +10018,7 @@
         <v>2016</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -10132,7 +10047,7 @@
         <v>2016</v>
       </c>
       <c r="I12" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -10161,12 +10076,12 @@
         <v>2016</v>
       </c>
       <c r="I13" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B14" s="3">
         <v>16112800000</v>
@@ -10190,12 +10105,12 @@
         <v>1956.8</v>
       </c>
       <c r="I14" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B15" s="3">
         <v>16341600000</v>
@@ -10219,12 +10134,12 @@
         <v>1967.1</v>
       </c>
       <c r="I15" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B16" s="3">
         <v>16570400000</v>
@@ -10248,12 +10163,12 @@
         <v>1977.4</v>
       </c>
       <c r="I16" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3">
         <v>16799200000</v>
@@ -10277,12 +10192,12 @@
         <v>1987.7</v>
       </c>
       <c r="I17" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B18" s="3">
         <v>17699000000</v>
@@ -10306,12 +10221,12 @@
         <v>2033</v>
       </c>
       <c r="I18" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B19" s="3">
         <v>16132000000</v>
@@ -10335,12 +10250,12 @@
         <v>1925</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B20" s="3">
         <v>17916000000</v>
@@ -10364,12 +10279,12 @@
         <v>2084</v>
       </c>
       <c r="I20" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3">
         <v>17544000000</v>
@@ -10393,12 +10308,12 @@
         <v>2008</v>
       </c>
       <c r="I21" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3">
         <v>18137000000</v>
@@ -10422,12 +10337,12 @@
         <v>2043</v>
       </c>
       <c r="I22" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3">
         <v>18843000000</v>
@@ -10451,12 +10366,12 @@
         <v>2084.5</v>
       </c>
       <c r="I23" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B24" s="3">
         <v>19407300000</v>
@@ -10480,12 +10395,12 @@
         <v>2112.3000000000002</v>
       </c>
       <c r="I24" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B25" s="3">
         <v>19971600000</v>
@@ -10509,7 +10424,7 @@
         <v>2140.1</v>
       </c>
       <c r="I25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix metadata table add suppression-flagging to data dict
</commit_message>
<xml_diff>
--- a/report-data-marts/monthly-milk-production/dummy-data/milk-prod-data-mart-reqs-1.5.xlsx
+++ b/report-data-marts/monthly-milk-production/dummy-data/milk-prod-data-mart-reqs-1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmartinez/Git/NASS-MILK/report-data-marts/monthly-milk-production/dummy-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9D2F83-2BF7-5343-9317-0A447A20E214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E867FB-CCFC-AF4B-ABDA-CBA7D0EF24CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3920" windowWidth="35840" windowHeight="18480" xr2:uid="{18E74043-749A-FF40-A645-80F0F71A40CB}"/>
+    <workbookView xWindow="0" yWindow="3920" windowWidth="35840" windowHeight="18480" activeTab="1" xr2:uid="{18E74043-749A-FF40-A645-80F0F71A40CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="94">
   <si>
     <t>Month</t>
   </si>
@@ -340,6 +340,15 @@
   </si>
   <si>
     <t>SURVEY</t>
+  </si>
+  <si>
+    <t>Suppressed</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Indicates if a NULL value in a column is NULL not because it is simply absent from the record, but because the value was suppressed for disclosure reasons. If no such column is in your data sample then none of your results included suppressed values.</t>
   </si>
 </sst>
 </file>
@@ -4150,7 +4159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384B1D2C-4EE8-4143-A35F-EB382FB4A755}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
@@ -5427,9 +5436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCDA15C-01AC-E947-8D92-BB3BD67D4DE6}">
   <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7618,7 +7625,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7627,17 +7634,12 @@
       <c r="A1" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>25</v>
-      </c>
+      <c r="B1" s="32"/>
       <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
       </c>
       <c r="C2" s="13"/>
     </row>
@@ -7660,7 +7662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57ABBB3-2F2C-DC44-81E7-671E85194010}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7815,12 +7819,19 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8467,7 +8478,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F20"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9692,9 +9703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC79A0EB-82C6-C948-BDEC-3E065A36834F}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I25"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
add aggregates as their own tables
</commit_message>
<xml_diff>
--- a/report-data-marts/monthly-milk-production/dummy-data/milk-prod-data-mart-reqs-1.5.xlsx
+++ b/report-data-marts/monthly-milk-production/dummy-data/milk-prod-data-mart-reqs-1.5.xlsx
@@ -8,23 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmartinez/Git/NASS-MILK/report-data-marts/monthly-milk-production/dummy-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E867FB-CCFC-AF4B-ABDA-CBA7D0EF24CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B307B21C-AB8D-5D4D-8630-6941E6486602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3920" windowWidth="35840" windowHeight="18480" activeTab="1" xr2:uid="{18E74043-749A-FF40-A645-80F0F71A40CB}"/>
+    <workbookView xWindow="14980" yWindow="3920" windowWidth="20860" windowHeight="18480" firstSheet="10" activeTab="13" xr2:uid="{18E74043-749A-FF40-A645-80F0F71A40CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="6" r:id="rId1"/>
     <sheet name="data-dictionary" sheetId="4" r:id="rId2"/>
     <sheet name="QtrNatWdYrsPrsntLst" sheetId="2" r:id="rId3"/>
-    <sheet name="QtrNatLngYrsPrsntLst" sheetId="7" r:id="rId4"/>
-    <sheet name="Mo24stWdYrsPrsntLst" sheetId="1" r:id="rId5"/>
-    <sheet name="Mo24stLngYrsPrsntLst" sheetId="5" r:id="rId6"/>
-    <sheet name="MoNtnlWdYrsPrsntLst" sheetId="17" r:id="rId7"/>
-    <sheet name="MoNtnlLngYrsPrsntLst" sheetId="20" r:id="rId8"/>
-    <sheet name="24stRprt-moWdYrsPrsntLst" sheetId="3" r:id="rId9"/>
-    <sheet name="24stRprt-lstmoWdYrsPrsntLst" sheetId="18" r:id="rId10"/>
-    <sheet name="24stRprtMnthsLngYrsPrsntLst" sheetId="21" r:id="rId11"/>
-    <sheet name="metadata" sheetId="8" r:id="rId12"/>
+    <sheet name="AggrQNWYPL" sheetId="22" r:id="rId4"/>
+    <sheet name="QtrNatLngYrsPrsntLst" sheetId="7" r:id="rId5"/>
+    <sheet name="Mo24stWdYrsPrsntLst" sheetId="1" r:id="rId6"/>
+    <sheet name="AggrM24sWYPL" sheetId="23" r:id="rId7"/>
+    <sheet name="Mo24stLngYrsPrsntLst" sheetId="5" r:id="rId8"/>
+    <sheet name="MoNtnlWdYrsPrsntLst" sheetId="17" r:id="rId9"/>
+    <sheet name="AggrNWYPL" sheetId="24" r:id="rId10"/>
+    <sheet name="MoNtnlLngYrsPrsntLst" sheetId="20" r:id="rId11"/>
+    <sheet name="24stRprt-moWdYrsPrsntLst" sheetId="3" r:id="rId12"/>
+    <sheet name="24stRprt-lstmoWdYrsPrsntLst" sheetId="18" r:id="rId13"/>
+    <sheet name="Aggr24sRmlWYPL" sheetId="25" r:id="rId14"/>
+    <sheet name="24stRprtMnthsLngYrsPrsntLst" sheetId="21" r:id="rId15"/>
+    <sheet name="metadata" sheetId="8" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="97">
   <si>
     <t>Month</t>
   </si>
@@ -350,11 +354,23 @@
   <si>
     <t>Indicates if a NULL value in a column is NULL not because it is simply absent from the record, but because the value was suppressed for disclosure reasons. If no such column is in your data sample then none of your results included suppressed values.</t>
   </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>24-States</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -546,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -604,6 +620,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4688,11 +4706,1257 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61152898-78E1-BF4C-A6C9-DAEFEFDDBD4C}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="84" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="3">
+        <v>218382</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3">
+        <v>9336</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>23391</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5ADF8FD-0B82-3D4D-A870-EF3E38E0C60C}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>17699000000</v>
+      </c>
+      <c r="B2" s="3">
+        <v>8805000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2010</v>
+      </c>
+      <c r="D2">
+        <v>2019</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>16132000000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>8803000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1833</v>
+      </c>
+      <c r="D3">
+        <v>2019</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>17916000000</v>
+      </c>
+      <c r="B4" s="3">
+        <v>8789000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2038</v>
+      </c>
+      <c r="D4">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>17544000000</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8788000</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1996</v>
+      </c>
+      <c r="D5">
+        <v>2019</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>18137000000</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8790000</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2063</v>
+      </c>
+      <c r="D6">
+        <v>2019</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>17342000000</v>
+      </c>
+      <c r="B7" s="3">
+        <v>8784000</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1974</v>
+      </c>
+      <c r="D7">
+        <v>2019</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>17542000000</v>
+      </c>
+      <c r="B8" s="3">
+        <v>8785000</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1997</v>
+      </c>
+      <c r="D8">
+        <v>2019</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>17439000000</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8789000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1984</v>
+      </c>
+      <c r="D9">
+        <v>2019</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>16796000000</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8805000</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1908</v>
+      </c>
+      <c r="D10">
+        <v>2019</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>17299000000</v>
+      </c>
+      <c r="B11" s="3">
+        <v>8819000</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1962</v>
+      </c>
+      <c r="D11">
+        <v>2019</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>16699000000</v>
+      </c>
+      <c r="B12" s="3">
+        <v>8817000</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1894</v>
+      </c>
+      <c r="D12">
+        <v>2019</v>
+      </c>
+      <c r="E12" s="1">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>17517000000</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8816000</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1987</v>
+      </c>
+      <c r="D13">
+        <v>2019</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>17956000000</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8834000</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2033</v>
+      </c>
+      <c r="D14">
+        <v>2020</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>17031000000</v>
+      </c>
+      <c r="B15" s="3">
+        <v>8848000</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1925</v>
+      </c>
+      <c r="D15">
+        <v>2020</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>18455000000</v>
+      </c>
+      <c r="B16" s="3">
+        <v>8857000</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2084</v>
+      </c>
+      <c r="D16">
+        <v>2020</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>17778000000</v>
+      </c>
+      <c r="B17" s="3">
+        <v>8852000</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2008</v>
+      </c>
+      <c r="D17">
+        <v>2020</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>18049000000</v>
+      </c>
+      <c r="B18" s="3">
+        <v>8836000</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2043</v>
+      </c>
+      <c r="D18">
+        <v>2020</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>17486000000</v>
+      </c>
+      <c r="B19" s="3">
+        <v>8827000</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1981</v>
+      </c>
+      <c r="D19">
+        <v>2020</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>17800000000</v>
+      </c>
+      <c r="B20" s="3">
+        <v>8829000</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2016</v>
+      </c>
+      <c r="D20">
+        <v>2020</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC79A0EB-82C6-C948-BDEC-3E065A36834F}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <v>17699000000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>17956000000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>8805000</v>
+      </c>
+      <c r="F2" s="3">
+        <v>8834000</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2010</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2033</v>
+      </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <v>16132000000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>17031000000</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8803000</v>
+      </c>
+      <c r="F3" s="3">
+        <v>8848000</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1833</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1925</v>
+      </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>17916000000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>18455000000</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8789000</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8857000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2038</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2084</v>
+      </c>
+      <c r="I4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>17544000000</v>
+      </c>
+      <c r="C5" s="3">
+        <v>17778000000</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>8788000</v>
+      </c>
+      <c r="F5" s="3">
+        <v>8852000</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1996</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2008</v>
+      </c>
+      <c r="I5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3">
+        <v>18137000000</v>
+      </c>
+      <c r="C6" s="3">
+        <v>18049000000</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>8790000</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8836000</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2063</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2043</v>
+      </c>
+      <c r="I6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>17342000000</v>
+      </c>
+      <c r="C7" s="3">
+        <v>17486000000</v>
+      </c>
+      <c r="D7" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>8784000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8827000</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1974</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1981</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>17542000000</v>
+      </c>
+      <c r="C8" s="3">
+        <v>17800000000</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>8785000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8829000</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1997</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2016</v>
+      </c>
+      <c r="I8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>17439000000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>17800000000</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8785000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8829000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1985</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2016</v>
+      </c>
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <v>16796000000</v>
+      </c>
+      <c r="C10" s="3">
+        <v>17800000000</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="E10" s="3">
+        <v>8785000</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8829000</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1912</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2016</v>
+      </c>
+      <c r="I10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3">
+        <v>17299000000</v>
+      </c>
+      <c r="C11" s="3">
+        <v>17800000000</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8785000</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8829000</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1969</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2016</v>
+      </c>
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
+        <v>16699000000</v>
+      </c>
+      <c r="C12" s="3">
+        <v>17800000000</v>
+      </c>
+      <c r="D12" s="4">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>8785000</v>
+      </c>
+      <c r="F12" s="3">
+        <v>8829000</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1901</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2016</v>
+      </c>
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>17517000000</v>
+      </c>
+      <c r="C13" s="3">
+        <v>17800000000</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8785000</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8829000</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1994</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2016</v>
+      </c>
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="3">
+        <v>16112800000</v>
+      </c>
+      <c r="C14" s="3">
+        <v>17294000000</v>
+      </c>
+      <c r="D14" s="4">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8822000</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8840600</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1826.6</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1956.8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="3">
+        <v>16341600000</v>
+      </c>
+      <c r="C15" s="3">
+        <v>17387300000</v>
+      </c>
+      <c r="D15" s="4">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>8817500</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8841400</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1853.5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1967.1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="3">
+        <v>16570400000</v>
+      </c>
+      <c r="C16" s="3">
+        <v>17480600000</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>8813000</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8842200</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1880.4</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1977.4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16799200000</v>
+      </c>
+      <c r="C17" s="3">
+        <v>17573900000</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4.6699999999999998E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>8808500</v>
+      </c>
+      <c r="F17" s="3">
+        <v>8843000</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1907.3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1987.7</v>
+      </c>
+      <c r="I17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="3">
+        <v>17699000000</v>
+      </c>
+      <c r="C18" s="3">
+        <v>17956000000</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>8805000</v>
+      </c>
+      <c r="F18" s="3">
+        <v>8834000</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2010</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2033</v>
+      </c>
+      <c r="I18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="3">
+        <v>16132000000</v>
+      </c>
+      <c r="C19" s="3">
+        <v>17031000000</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>8803000</v>
+      </c>
+      <c r="F19" s="3">
+        <v>8848000</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1833</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1925</v>
+      </c>
+      <c r="I19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="3">
+        <v>17916000000</v>
+      </c>
+      <c r="C20" s="3">
+        <v>18455000000</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E20" s="3">
+        <v>8789000</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8857000</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2038</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2084</v>
+      </c>
+      <c r="I20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="3">
+        <v>17544000000</v>
+      </c>
+      <c r="C21" s="3">
+        <v>17778000000</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>8788000</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8852000</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1996</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2008</v>
+      </c>
+      <c r="I21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="3">
+        <v>18137000000</v>
+      </c>
+      <c r="C22" s="3">
+        <v>18049000000</v>
+      </c>
+      <c r="D22" s="4">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8790000</v>
+      </c>
+      <c r="F22" s="3">
+        <v>8836000</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2063</v>
+      </c>
+      <c r="H22" s="3">
+        <v>2043</v>
+      </c>
+      <c r="I22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="3">
+        <v>18843000000</v>
+      </c>
+      <c r="C23" s="3">
+        <v>18422500000</v>
+      </c>
+      <c r="D23" s="4">
+        <v>-2.6499999999999999E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>8782500</v>
+      </c>
+      <c r="F23" s="3">
+        <v>8838000</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2144.5</v>
+      </c>
+      <c r="H23" s="3">
+        <v>2084.5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="3">
+        <v>19407300000</v>
+      </c>
+      <c r="C24" s="3">
+        <v>18660200000</v>
+      </c>
+      <c r="D24" s="4">
+        <v>-4.65E-2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>8778500</v>
+      </c>
+      <c r="F24" s="3">
+        <v>8833900</v>
+      </c>
+      <c r="G24" s="3">
+        <v>2209.3000000000002</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2112.3000000000002</v>
+      </c>
+      <c r="I24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="3">
+        <v>19971600000</v>
+      </c>
+      <c r="C25" s="3">
+        <v>18897900000</v>
+      </c>
+      <c r="D25" s="4">
+        <v>-6.6500000000000004E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>8774500</v>
+      </c>
+      <c r="F25" s="3">
+        <v>8829800</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2274.1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>2140.1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4198FD-6C2A-B444-853F-C699E2177104}">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5432,7 +6696,113 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3A40A3-B37B-A54E-9A92-21AE1B6E1EF6}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="33">
+        <v>17439</v>
+      </c>
+      <c r="C2" s="33">
+        <v>17763</v>
+      </c>
+      <c r="D2" s="34">
+        <v>1.9</v>
+      </c>
+      <c r="E2" s="33">
+        <v>8789</v>
+      </c>
+      <c r="F2" s="33">
+        <v>8840</v>
+      </c>
+      <c r="G2" s="33">
+        <v>1984</v>
+      </c>
+      <c r="H2" s="33">
+        <v>2009</v>
+      </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="33">
+        <v>17542</v>
+      </c>
+      <c r="C3" s="33">
+        <v>17891</v>
+      </c>
+      <c r="D3" s="34">
+        <v>2</v>
+      </c>
+      <c r="E3" s="33">
+        <v>8785</v>
+      </c>
+      <c r="F3" s="33">
+        <v>8840</v>
+      </c>
+      <c r="G3" s="33">
+        <v>1997</v>
+      </c>
+      <c r="H3" s="33">
+        <v>2024</v>
+      </c>
+      <c r="I3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCDA15C-01AC-E947-8D92-BB3BD67D4DE6}">
   <dimension ref="A1:T97"/>
   <sheetViews>
@@ -7620,7 +8990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF68689-30C7-074E-8257-973C71620241}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -7662,7 +9032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57ABBB3-2F2C-DC44-81E7-671E85194010}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -7840,7 +9210,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7968,6 +9338,66 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E4F694-F7C6-7F48-B1B6-864A894691BC}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="84" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="3">
+        <v>218382</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3">
+        <v>9336</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>23391</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C6F5B0-0C81-0D41-9D0F-91912B57482A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -8109,12 +9539,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6E745E-4567-8043-A8D2-827598A83DCD}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8473,7 +9903,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19866B47-7931-EA4F-84EA-6AB70F62424F}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="3">
+        <v>208062</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3">
+        <v>8799</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>23646</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A268244C-A828-FB4A-BC13-67F19F7381C2}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -8894,7 +10386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E096290-E173-4B42-A453-82A947F07FF4}">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -9256,1188 +10748,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5ADF8FD-0B82-3D4D-A870-EF3E38E0C60C}">
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="42" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>17699000000</v>
-      </c>
-      <c r="B2" s="3">
-        <v>8805000</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2010</v>
-      </c>
-      <c r="D2">
-        <v>2019</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>16132000000</v>
-      </c>
-      <c r="B3" s="3">
-        <v>8803000</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1833</v>
-      </c>
-      <c r="D3">
-        <v>2019</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>17916000000</v>
-      </c>
-      <c r="B4" s="3">
-        <v>8789000</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2038</v>
-      </c>
-      <c r="D4">
-        <v>2019</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>17544000000</v>
-      </c>
-      <c r="B5" s="3">
-        <v>8788000</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1996</v>
-      </c>
-      <c r="D5">
-        <v>2019</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>18137000000</v>
-      </c>
-      <c r="B6" s="3">
-        <v>8790000</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2063</v>
-      </c>
-      <c r="D6">
-        <v>2019</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>17342000000</v>
-      </c>
-      <c r="B7" s="3">
-        <v>8784000</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1974</v>
-      </c>
-      <c r="D7">
-        <v>2019</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>17542000000</v>
-      </c>
-      <c r="B8" s="3">
-        <v>8785000</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1997</v>
-      </c>
-      <c r="D8">
-        <v>2019</v>
-      </c>
-      <c r="E8" s="1">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>17439000000</v>
-      </c>
-      <c r="B9" s="3">
-        <v>8789000</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1984</v>
-      </c>
-      <c r="D9">
-        <v>2019</v>
-      </c>
-      <c r="E9" s="1">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>16796000000</v>
-      </c>
-      <c r="B10" s="3">
-        <v>8805000</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1908</v>
-      </c>
-      <c r="D10">
-        <v>2019</v>
-      </c>
-      <c r="E10" s="1">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>17299000000</v>
-      </c>
-      <c r="B11" s="3">
-        <v>8819000</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1962</v>
-      </c>
-      <c r="D11">
-        <v>2019</v>
-      </c>
-      <c r="E11" s="1">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>16699000000</v>
-      </c>
-      <c r="B12" s="3">
-        <v>8817000</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1894</v>
-      </c>
-      <c r="D12">
-        <v>2019</v>
-      </c>
-      <c r="E12" s="1">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>17517000000</v>
-      </c>
-      <c r="B13" s="3">
-        <v>8816000</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1987</v>
-      </c>
-      <c r="D13">
-        <v>2019</v>
-      </c>
-      <c r="E13" s="1">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>17956000000</v>
-      </c>
-      <c r="B14" s="3">
-        <v>8834000</v>
-      </c>
-      <c r="C14" s="3">
-        <v>2033</v>
-      </c>
-      <c r="D14">
-        <v>2020</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>17031000000</v>
-      </c>
-      <c r="B15" s="3">
-        <v>8848000</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1925</v>
-      </c>
-      <c r="D15">
-        <v>2020</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>18455000000</v>
-      </c>
-      <c r="B16" s="3">
-        <v>8857000</v>
-      </c>
-      <c r="C16" s="3">
-        <v>2084</v>
-      </c>
-      <c r="D16">
-        <v>2020</v>
-      </c>
-      <c r="E16" s="1">
-        <v>3</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>17778000000</v>
-      </c>
-      <c r="B17" s="3">
-        <v>8852000</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2008</v>
-      </c>
-      <c r="D17">
-        <v>2020</v>
-      </c>
-      <c r="E17" s="1">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>18049000000</v>
-      </c>
-      <c r="B18" s="3">
-        <v>8836000</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2043</v>
-      </c>
-      <c r="D18">
-        <v>2020</v>
-      </c>
-      <c r="E18" s="1">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>17486000000</v>
-      </c>
-      <c r="B19" s="3">
-        <v>8827000</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1981</v>
-      </c>
-      <c r="D19">
-        <v>2020</v>
-      </c>
-      <c r="E19" s="1">
-        <v>6</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>17800000000</v>
-      </c>
-      <c r="B20" s="3">
-        <v>8829000</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2016</v>
-      </c>
-      <c r="D20">
-        <v>2020</v>
-      </c>
-      <c r="E20" s="1">
-        <v>7</v>
-      </c>
-      <c r="F20" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC79A0EB-82C6-C948-BDEC-3E065A36834F}">
-  <dimension ref="A1:I25"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="84" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3">
-        <v>17699000000</v>
-      </c>
-      <c r="C2" s="3">
-        <v>17956000000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>8805000</v>
-      </c>
-      <c r="F2" s="3">
-        <v>8834000</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2010</v>
-      </c>
-      <c r="H2" s="3">
-        <v>2033</v>
-      </c>
-      <c r="I2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3">
-        <v>16132000000</v>
-      </c>
-      <c r="C3" s="3">
-        <v>17031000000</v>
-      </c>
-      <c r="D3" s="4">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>8803000</v>
-      </c>
-      <c r="F3" s="3">
-        <v>8848000</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1833</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1925</v>
-      </c>
-      <c r="I3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3">
-        <v>17916000000</v>
-      </c>
-      <c r="C4" s="3">
-        <v>18455000000</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="E4" s="3">
-        <v>8789000</v>
-      </c>
-      <c r="F4" s="3">
-        <v>8857000</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2038</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2084</v>
-      </c>
-      <c r="I4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3">
-        <v>17544000000</v>
-      </c>
-      <c r="C5" s="3">
-        <v>17778000000</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>8788000</v>
-      </c>
-      <c r="F5" s="3">
-        <v>8852000</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1996</v>
-      </c>
-      <c r="H5" s="3">
-        <v>2008</v>
-      </c>
-      <c r="I5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3">
-        <v>18137000000</v>
-      </c>
-      <c r="C6" s="3">
-        <v>18049000000</v>
-      </c>
-      <c r="D6" s="4">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="E6" s="3">
-        <v>8790000</v>
-      </c>
-      <c r="F6" s="3">
-        <v>8836000</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2063</v>
-      </c>
-      <c r="H6" s="3">
-        <v>2043</v>
-      </c>
-      <c r="I6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3">
-        <v>17342000000</v>
-      </c>
-      <c r="C7" s="3">
-        <v>17486000000</v>
-      </c>
-      <c r="D7" s="4">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E7" s="3">
-        <v>8784000</v>
-      </c>
-      <c r="F7" s="3">
-        <v>8827000</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1974</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1981</v>
-      </c>
-      <c r="I7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3">
-        <v>17542000000</v>
-      </c>
-      <c r="C8" s="3">
-        <v>17800000000</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>8785000</v>
-      </c>
-      <c r="F8" s="3">
-        <v>8829000</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1997</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2016</v>
-      </c>
-      <c r="I8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3">
-        <v>17439000000</v>
-      </c>
-      <c r="C9" s="3">
-        <v>17800000000</v>
-      </c>
-      <c r="D9" s="4">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>8785000</v>
-      </c>
-      <c r="F9" s="3">
-        <v>8829000</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1985</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2016</v>
-      </c>
-      <c r="I9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3">
-        <v>16796000000</v>
-      </c>
-      <c r="C10" s="3">
-        <v>17800000000</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="E10" s="3">
-        <v>8785000</v>
-      </c>
-      <c r="F10" s="3">
-        <v>8829000</v>
-      </c>
-      <c r="G10" s="3">
-        <v>1912</v>
-      </c>
-      <c r="H10" s="3">
-        <v>2016</v>
-      </c>
-      <c r="I10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3">
-        <v>17299000000</v>
-      </c>
-      <c r="C11" s="3">
-        <v>17800000000</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="E11" s="3">
-        <v>8785000</v>
-      </c>
-      <c r="F11" s="3">
-        <v>8829000</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1969</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2016</v>
-      </c>
-      <c r="I11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3">
-        <v>16699000000</v>
-      </c>
-      <c r="C12" s="3">
-        <v>17800000000</v>
-      </c>
-      <c r="D12" s="4">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>8785000</v>
-      </c>
-      <c r="F12" s="3">
-        <v>8829000</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1901</v>
-      </c>
-      <c r="H12" s="3">
-        <v>2016</v>
-      </c>
-      <c r="I12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3">
-        <v>17517000000</v>
-      </c>
-      <c r="C13" s="3">
-        <v>17800000000</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.6E-2</v>
-      </c>
-      <c r="E13" s="3">
-        <v>8785000</v>
-      </c>
-      <c r="F13" s="3">
-        <v>8829000</v>
-      </c>
-      <c r="G13" s="3">
-        <v>1994</v>
-      </c>
-      <c r="H13" s="3">
-        <v>2016</v>
-      </c>
-      <c r="I13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="3">
-        <v>16112800000</v>
-      </c>
-      <c r="C14" s="3">
-        <v>17294000000</v>
-      </c>
-      <c r="D14" s="4">
-        <v>7.1599999999999997E-2</v>
-      </c>
-      <c r="E14" s="3">
-        <v>8822000</v>
-      </c>
-      <c r="F14" s="3">
-        <v>8840600</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1826.6</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1956.8</v>
-      </c>
-      <c r="I14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="3">
-        <v>16341600000</v>
-      </c>
-      <c r="C15" s="3">
-        <v>17387300000</v>
-      </c>
-      <c r="D15" s="4">
-        <v>6.3299999999999995E-2</v>
-      </c>
-      <c r="E15" s="3">
-        <v>8817500</v>
-      </c>
-      <c r="F15" s="3">
-        <v>8841400</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1853.5</v>
-      </c>
-      <c r="H15" s="3">
-        <v>1967.1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="3">
-        <v>16570400000</v>
-      </c>
-      <c r="C16" s="3">
-        <v>17480600000</v>
-      </c>
-      <c r="D16" s="4">
-        <v>5.5E-2</v>
-      </c>
-      <c r="E16" s="3">
-        <v>8813000</v>
-      </c>
-      <c r="F16" s="3">
-        <v>8842200</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1880.4</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1977.4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="3">
-        <v>16799200000</v>
-      </c>
-      <c r="C17" s="3">
-        <v>17573900000</v>
-      </c>
-      <c r="D17" s="4">
-        <v>4.6699999999999998E-2</v>
-      </c>
-      <c r="E17" s="3">
-        <v>8808500</v>
-      </c>
-      <c r="F17" s="3">
-        <v>8843000</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1907.3</v>
-      </c>
-      <c r="H17" s="3">
-        <v>1987.7</v>
-      </c>
-      <c r="I17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="3">
-        <v>17699000000</v>
-      </c>
-      <c r="C18" s="3">
-        <v>17956000000</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E18" s="3">
-        <v>8805000</v>
-      </c>
-      <c r="F18" s="3">
-        <v>8834000</v>
-      </c>
-      <c r="G18" s="3">
-        <v>2010</v>
-      </c>
-      <c r="H18" s="3">
-        <v>2033</v>
-      </c>
-      <c r="I18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="3">
-        <v>16132000000</v>
-      </c>
-      <c r="C19" s="3">
-        <v>17031000000</v>
-      </c>
-      <c r="D19" s="4">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>8803000</v>
-      </c>
-      <c r="F19" s="3">
-        <v>8848000</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1833</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1925</v>
-      </c>
-      <c r="I19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="3">
-        <v>17916000000</v>
-      </c>
-      <c r="C20" s="3">
-        <v>18455000000</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="E20" s="3">
-        <v>8789000</v>
-      </c>
-      <c r="F20" s="3">
-        <v>8857000</v>
-      </c>
-      <c r="G20" s="3">
-        <v>2038</v>
-      </c>
-      <c r="H20" s="3">
-        <v>2084</v>
-      </c>
-      <c r="I20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="3">
-        <v>17544000000</v>
-      </c>
-      <c r="C21" s="3">
-        <v>17778000000</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E21" s="3">
-        <v>8788000</v>
-      </c>
-      <c r="F21" s="3">
-        <v>8852000</v>
-      </c>
-      <c r="G21" s="3">
-        <v>1996</v>
-      </c>
-      <c r="H21" s="3">
-        <v>2008</v>
-      </c>
-      <c r="I21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="3">
-        <v>18137000000</v>
-      </c>
-      <c r="C22" s="3">
-        <v>18049000000</v>
-      </c>
-      <c r="D22" s="4">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="E22" s="3">
-        <v>8790000</v>
-      </c>
-      <c r="F22" s="3">
-        <v>8836000</v>
-      </c>
-      <c r="G22" s="3">
-        <v>2063</v>
-      </c>
-      <c r="H22" s="3">
-        <v>2043</v>
-      </c>
-      <c r="I22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="3">
-        <v>18843000000</v>
-      </c>
-      <c r="C23" s="3">
-        <v>18422500000</v>
-      </c>
-      <c r="D23" s="4">
-        <v>-2.6499999999999999E-2</v>
-      </c>
-      <c r="E23" s="3">
-        <v>8782500</v>
-      </c>
-      <c r="F23" s="3">
-        <v>8838000</v>
-      </c>
-      <c r="G23" s="3">
-        <v>2144.5</v>
-      </c>
-      <c r="H23" s="3">
-        <v>2084.5</v>
-      </c>
-      <c r="I23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="3">
-        <v>19407300000</v>
-      </c>
-      <c r="C24" s="3">
-        <v>18660200000</v>
-      </c>
-      <c r="D24" s="4">
-        <v>-4.65E-2</v>
-      </c>
-      <c r="E24" s="3">
-        <v>8778500</v>
-      </c>
-      <c r="F24" s="3">
-        <v>8833900</v>
-      </c>
-      <c r="G24" s="3">
-        <v>2209.3000000000002</v>
-      </c>
-      <c r="H24" s="3">
-        <v>2112.3000000000002</v>
-      </c>
-      <c r="I24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="3">
-        <v>19971600000</v>
-      </c>
-      <c r="C25" s="3">
-        <v>18897900000</v>
-      </c>
-      <c r="D25" s="4">
-        <v>-6.6500000000000004E-2</v>
-      </c>
-      <c r="E25" s="3">
-        <v>8774500</v>
-      </c>
-      <c r="F25" s="3">
-        <v>8829800</v>
-      </c>
-      <c r="G25" s="3">
-        <v>2274.1</v>
-      </c>
-      <c r="H25" s="3">
-        <v>2140.1</v>
-      </c>
-      <c r="I25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>